<commit_message>
crossed out codes not useful
</commit_message>
<xml_diff>
--- a/results/output_unified_duration.xlsx
+++ b/results/output_unified_duration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/semiauto-epi-data-extraction-pipeline/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2112A18E-6238-8B43-BBE1-D5BE06639006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1384D6B5-CC24-3647-8EF7-9CEECD5527AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1602,15 +1602,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="CW22" sqref="CW22"/>
+    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="AZ22" sqref="AZ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="96" max="96" width="42.5" customWidth="1"/>
-    <col min="98" max="98" width="25" customWidth="1"/>
-    <col min="99" max="99" width="24" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="29" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="37" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="42" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="146.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="105.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="102" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="24" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="60" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="64" width="49" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="51" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="56" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="63.83203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="53" bestFit="1" customWidth="1"/>
+    <col min="81" max="82" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="64" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="63.83203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="57" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="99.5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="89.33203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="84.1640625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
merged funcs to parse ages stats into main func
</commit_message>
<xml_diff>
--- a/results/output_unified_duration.xlsx
+++ b/results/output_unified_duration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/DS_Projects/semiauto-epi-data-extraction-pipeline/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1384D6B5-CC24-3647-8EF7-9CEECD5527AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B3FB5-2AEB-2F45-832A-709C6CF2B298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="AZ22" sqref="AZ22"/>
+    <sheetView tabSelected="1" topLeftCell="CP1" workbookViewId="0">
+      <selection activeCell="CX17" sqref="CX17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>